<commit_message>
Update Requisitos de sistema.xlsx
</commit_message>
<xml_diff>
--- a/Requisitos de sistema.xlsx
+++ b/Requisitos de sistema.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21601"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\proyecto\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Cristian\Documents\GitHub\Proyecto_Hipermedial\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9FC81B5E-9136-40DB-B88C-FECA4B9EB077}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24DDB4F4-18B8-4203-9A03-014D925F8CB4}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20496" windowHeight="7548" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="19392" windowHeight="10536" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Plantilla de matriz requisitos" sheetId="1" r:id="rId1"/>
@@ -427,9 +427,6 @@
     <t>R-35</t>
   </si>
   <si>
-    <t>Cancelar pedidod</t>
-  </si>
-  <si>
     <t>Poder cancelar un pedido para posteriormente solicitar un reembolso en caso se lleve a cabo correctamente</t>
   </si>
   <si>
@@ -488,6 +485,9 @@
   </si>
   <si>
     <t>Adminstrador de Usuario, Usuario</t>
+  </si>
+  <si>
+    <t>Cancelar pedidos</t>
   </si>
 </sst>
 </file>
@@ -587,7 +587,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -909,25 +909,25 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H42"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" zoomScalePageLayoutView="70" workbookViewId="0">
-      <selection activeCell="G49" sqref="G49"/>
+    <sheetView tabSelected="1" topLeftCell="A31" zoomScale="70" zoomScaleNormal="70" zoomScalePageLayoutView="70" workbookViewId="0">
+      <selection activeCell="C41" sqref="C41"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="11.41796875" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="1" width="14.6640625" style="1" customWidth="1"/>
+    <col min="1" max="1" width="14.68359375" style="1" customWidth="1"/>
     <col min="2" max="2" width="42" style="1" customWidth="1"/>
-    <col min="3" max="3" width="26.5546875" style="1" customWidth="1"/>
-    <col min="4" max="4" width="62.5546875" style="3" customWidth="1"/>
-    <col min="5" max="5" width="26.5546875" style="1" customWidth="1"/>
-    <col min="6" max="6" width="30.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="26.6640625" style="1" customWidth="1"/>
-    <col min="8" max="8" width="21.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="32.44140625" style="1" customWidth="1"/>
-    <col min="10" max="16384" width="11.44140625" style="1"/>
+    <col min="3" max="3" width="26.5234375" style="1" customWidth="1"/>
+    <col min="4" max="4" width="62.5234375" style="3" customWidth="1"/>
+    <col min="5" max="5" width="26.5234375" style="1" customWidth="1"/>
+    <col min="6" max="6" width="30.3125" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="26.68359375" style="1" customWidth="1"/>
+    <col min="8" max="8" width="21.68359375" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="32.41796875" style="1" customWidth="1"/>
+    <col min="10" max="16384" width="11.41796875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -953,7 +953,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" s="4" t="s">
         <v>11</v>
       </c>
@@ -979,7 +979,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" s="4" t="s">
         <v>12</v>
       </c>
@@ -1005,7 +1005,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" s="4" t="s">
         <v>13</v>
       </c>
@@ -1031,7 +1031,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="5" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" s="4" t="s">
         <v>14</v>
       </c>
@@ -1057,7 +1057,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="6" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" s="4" t="s">
         <v>15</v>
       </c>
@@ -1083,7 +1083,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="7" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" s="4" t="s">
         <v>16</v>
       </c>
@@ -1109,7 +1109,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="8" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" s="4" t="s">
         <v>17</v>
       </c>
@@ -1135,7 +1135,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="9" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" s="4" t="s">
         <v>18</v>
       </c>
@@ -1161,7 +1161,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="10" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" s="4" t="s">
         <v>19</v>
       </c>
@@ -1187,7 +1187,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="11" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" s="4" t="s">
         <v>20</v>
       </c>
@@ -1213,7 +1213,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="12" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A12" s="4" t="s">
         <v>21</v>
       </c>
@@ -1239,7 +1239,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="13" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A13" s="4" t="s">
         <v>22</v>
       </c>
@@ -1265,7 +1265,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="14" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A14" s="4" t="s">
         <v>23</v>
       </c>
@@ -1291,7 +1291,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="15" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:8" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A15" s="4" t="s">
         <v>52</v>
       </c>
@@ -1317,7 +1317,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A16" s="4" t="s">
         <v>53</v>
       </c>
@@ -1343,7 +1343,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="17" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:8" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A17" s="4" t="s">
         <v>54</v>
       </c>
@@ -1369,7 +1369,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="18" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:8" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A18" s="4" t="s">
         <v>55</v>
       </c>
@@ -1395,7 +1395,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="19" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:8" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A19" s="4" t="s">
         <v>56</v>
       </c>
@@ -1421,7 +1421,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="20" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:8" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A20" s="4" t="s">
         <v>57</v>
       </c>
@@ -1447,7 +1447,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="21" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:8" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A21" s="4" t="s">
         <v>58</v>
       </c>
@@ -1473,7 +1473,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="22" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:8" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A22" s="4" t="s">
         <v>59</v>
       </c>
@@ -1499,7 +1499,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="23" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:8" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A23" s="4" t="s">
         <v>60</v>
       </c>
@@ -1525,7 +1525,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="24" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:8" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A24" s="4" t="s">
         <v>61</v>
       </c>
@@ -1551,7 +1551,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="25" spans="1:8" ht="44.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:8" ht="44.25" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A25" s="4" t="s">
         <v>62</v>
       </c>
@@ -1577,7 +1577,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="26" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:8" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A26" s="4" t="s">
         <v>63</v>
       </c>
@@ -1603,7 +1603,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="27" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:8" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A27" s="4" t="s">
         <v>64</v>
       </c>
@@ -1629,7 +1629,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="28" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:8" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A28" s="4" t="s">
         <v>65</v>
       </c>
@@ -1655,7 +1655,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="29" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:8" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A29" s="4" t="s">
         <v>66</v>
       </c>
@@ -1681,7 +1681,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="30" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:8" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A30" s="4" t="s">
         <v>67</v>
       </c>
@@ -1707,7 +1707,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="31" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:8" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A31" s="4" t="s">
         <v>68</v>
       </c>
@@ -1733,7 +1733,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="32" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:8" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A32" s="4" t="s">
         <v>69</v>
       </c>
@@ -1759,7 +1759,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="33" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A33" s="4" t="s">
         <v>70</v>
       </c>
@@ -1785,7 +1785,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="34" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:8" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A34" s="4" t="s">
         <v>71</v>
       </c>
@@ -1811,7 +1811,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="35" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:8" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A35" s="4" t="s">
         <v>129</v>
       </c>
@@ -1819,7 +1819,7 @@
         <v>130</v>
       </c>
       <c r="C35" s="4" t="s">
-        <v>8</v>
+        <v>98</v>
       </c>
       <c r="D35" s="4" t="s">
         <v>131</v>
@@ -1837,18 +1837,18 @@
         <v>125</v>
       </c>
     </row>
-    <row r="36" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:8" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A36" s="4" t="s">
         <v>132</v>
       </c>
       <c r="B36" s="4" t="s">
+        <v>153</v>
+      </c>
+      <c r="C36" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="D36" s="4" t="s">
         <v>133</v>
-      </c>
-      <c r="C36" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="D36" s="4" t="s">
-        <v>134</v>
       </c>
       <c r="E36" s="4" t="s">
         <v>27</v>
@@ -1863,18 +1863,18 @@
         <v>125</v>
       </c>
     </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A37" s="4" t="s">
+        <v>134</v>
+      </c>
+      <c r="B37" s="4" t="s">
         <v>135</v>
       </c>
-      <c r="B37" s="4" t="s">
+      <c r="C37" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="D37" s="4" t="s">
         <v>136</v>
-      </c>
-      <c r="C37" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="D37" s="4" t="s">
-        <v>137</v>
       </c>
       <c r="E37" s="4" t="s">
         <v>10</v>
@@ -1889,18 +1889,18 @@
         <v>125</v>
       </c>
     </row>
-    <row r="38" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:8" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A38" s="4" t="s">
+        <v>137</v>
+      </c>
+      <c r="B38" s="4" t="s">
         <v>138</v>
       </c>
-      <c r="B38" s="4" t="s">
+      <c r="C38" s="4" t="s">
         <v>139</v>
       </c>
-      <c r="C38" s="4" t="s">
+      <c r="D38" s="4" t="s">
         <v>140</v>
-      </c>
-      <c r="D38" s="4" t="s">
-        <v>141</v>
       </c>
       <c r="E38" s="4" t="s">
         <v>26</v>
@@ -1915,18 +1915,18 @@
         <v>127</v>
       </c>
     </row>
-    <row r="39" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:8" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A39" s="4" t="s">
+        <v>141</v>
+      </c>
+      <c r="B39" s="4" t="s">
         <v>142</v>
       </c>
-      <c r="B39" s="4" t="s">
+      <c r="C39" s="4" t="s">
+        <v>139</v>
+      </c>
+      <c r="D39" s="4" t="s">
         <v>143</v>
-      </c>
-      <c r="C39" s="4" t="s">
-        <v>140</v>
-      </c>
-      <c r="D39" s="4" t="s">
-        <v>144</v>
       </c>
       <c r="E39" s="4" t="s">
         <v>26</v>
@@ -1941,18 +1941,18 @@
         <v>125</v>
       </c>
     </row>
-    <row r="40" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:8" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A40" s="4" t="s">
+        <v>144</v>
+      </c>
+      <c r="B40" s="4" t="s">
         <v>145</v>
       </c>
-      <c r="B40" s="4" t="s">
+      <c r="C40" s="4" t="s">
+        <v>139</v>
+      </c>
+      <c r="D40" s="4" t="s">
         <v>146</v>
-      </c>
-      <c r="C40" s="4" t="s">
-        <v>140</v>
-      </c>
-      <c r="D40" s="4" t="s">
-        <v>147</v>
       </c>
       <c r="E40" s="4" t="s">
         <v>27</v>
@@ -1967,18 +1967,18 @@
         <v>125</v>
       </c>
     </row>
-    <row r="41" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:8" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A41" s="4" t="s">
+        <v>147</v>
+      </c>
+      <c r="B41" s="4" t="s">
         <v>148</v>
       </c>
-      <c r="B41" s="4" t="s">
+      <c r="C41" s="4" t="s">
+        <v>139</v>
+      </c>
+      <c r="D41" s="4" t="s">
         <v>149</v>
-      </c>
-      <c r="C41" s="4" t="s">
-        <v>140</v>
-      </c>
-      <c r="D41" s="4" t="s">
-        <v>150</v>
       </c>
       <c r="E41" s="4" t="s">
         <v>27</v>
@@ -1993,24 +1993,24 @@
         <v>125</v>
       </c>
     </row>
-    <row r="42" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:8" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A42" s="4" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B42" s="4" t="s">
+        <v>150</v>
+      </c>
+      <c r="C42" s="4" t="s">
+        <v>139</v>
+      </c>
+      <c r="D42" s="4" t="s">
         <v>151</v>
       </c>
-      <c r="C42" s="4" t="s">
-        <v>140</v>
-      </c>
-      <c r="D42" s="4" t="s">
+      <c r="E42" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="F42" s="4" t="s">
         <v>152</v>
-      </c>
-      <c r="E42" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="F42" s="4" t="s">
-        <v>153</v>
       </c>
       <c r="G42" s="4" t="s">
         <v>10</v>

</xml_diff>